<commit_message>
Extensive update to integrate windfarm into docs
Now there is a windfarm permanently but if it (or the PV plant) is not selected in the main doc, the availability is set to 0, effectively disabling it.
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base_methanol.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base_methanol.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/methanol/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="13_ncr:1_{D954787A-120F-4E9B-9D31-96F6A5AD2E25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F32438C7-CED9-4A43-8C2C-454661B54E46}"/>
+  <xr:revisionPtr revIDLastSave="106" documentId="13_ncr:1_{D954787A-120F-4E9B-9D31-96F6A5AD2E25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67D31FD7-AF8F-4370-8CB6-70E1B85EF52A}"/>
   <bookViews>
-    <workbookView xWindow="-22815" yWindow="-21720" windowWidth="51840" windowHeight="21240" activeTab="3" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-22815" yWindow="-21720" windowWidth="51840" windowHeight="21240" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Drop_Down" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="CIQWBGuid" hidden="1">"a4f43e6a-2fed-40b8-8442-1e884dace181"</definedName>
+    <definedName name="CIQWBGuid" hidden="1">"c85e64f1-cccd-444b-83b1-b265e1061f52"</definedName>
     <definedName name="CIQWBInfo" hidden="1">"{ ""CIQVersion"":""9.51.3510.3078"" }"</definedName>
     <definedName name="IQ_CH">110000</definedName>
     <definedName name="IQ_CQ">5000</definedName>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="112">
   <si>
     <t>Unit</t>
   </si>
@@ -183,9 +183,6 @@
     <t>Error messages:</t>
   </si>
   <si>
-    <t>Solar_Plant_Kasso</t>
-  </si>
-  <si>
     <t>Power_Kasso</t>
   </si>
   <si>
@@ -403,6 +400,15 @@
   </si>
   <si>
     <t>Destilation_tower</t>
+  </si>
+  <si>
+    <t>Solar_Plant</t>
+  </si>
+  <si>
+    <t>Wind_Farm</t>
+  </si>
+  <si>
+    <t>Wind_farm</t>
   </si>
 </sst>
 </file>
@@ -551,8 +557,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:AQ7" totalsRowShown="0">
-  <autoFilter ref="A1:AQ7" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:AQ8" totalsRowShown="0">
+  <autoFilter ref="A1:AQ8" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
   <tableColumns count="43">
     <tableColumn id="1" xr3:uid="{C73E51D0-1842-42F3-9C00-F0DBD2E661BE}" name="Unit"/>
     <tableColumn id="40" xr3:uid="{C2CFC5A4-5329-4F74-926A-18CEB18C062C}" name="Object_type"/>
@@ -665,8 +671,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E5F8A7EB-52A6-4AC4-94D0-FF5952E382A3}" name="Table4" displayName="Table4" ref="A1:A16" totalsRowShown="0">
-  <autoFilter ref="A1:A16" xr:uid="{E5F8A7EB-52A6-4AC4-94D0-FF5952E382A3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E5F8A7EB-52A6-4AC4-94D0-FF5952E382A3}" name="Table4" displayName="Table4" ref="A1:A17" totalsRowShown="0">
+  <autoFilter ref="A1:A17" xr:uid="{E5F8A7EB-52A6-4AC4-94D0-FF5952E382A3}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{99EC3AFF-E76A-4BF2-94D0-13EEEC46286A}" name="object_type"/>
   </tableColumns>
@@ -971,10 +977,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
-  <dimension ref="A1:AQ9"/>
+  <dimension ref="A1:AQ8"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="Q29" sqref="Q29"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1013,7 +1019,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1094,7 +1100,7 @@
         <v>26</v>
       </c>
       <c r="AC1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AD1" t="s">
         <v>27</v>
@@ -1121,19 +1127,19 @@
         <v>34</v>
       </c>
       <c r="AL1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AM1" t="s">
         <v>75</v>
       </c>
-      <c r="AM1" t="s">
-        <v>76</v>
-      </c>
       <c r="AN1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AO1" t="s">
         <v>90</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>91</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>92</v>
       </c>
       <c r="AQ1" s="1" t="s">
         <v>35</v>
@@ -1141,13 +1147,13 @@
     </row>
     <row r="2" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" t="s">
         <v>36</v>
-      </c>
-      <c r="B2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E2" t="s">
-        <v>37</v>
       </c>
       <c r="K2">
         <v>304</v>
@@ -1165,10 +1171,10 @@
       <c r="AL2" s="3"/>
       <c r="AM2" s="3"/>
       <c r="AN2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AO2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AP2" s="5">
         <v>0</v>
@@ -1177,22 +1183,22 @@
     </row>
     <row r="3" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" t="s">
         <v>38</v>
       </c>
-      <c r="B3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>39</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>40</v>
-      </c>
-      <c r="F3" t="s">
-        <v>41</v>
       </c>
       <c r="G3">
         <v>52</v>
@@ -1221,10 +1227,10 @@
       <c r="AL3" s="3"/>
       <c r="AM3" s="3"/>
       <c r="AN3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AO3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AP3" s="5">
         <v>0</v>
@@ -1233,19 +1239,19 @@
     </row>
     <row r="4" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" t="s">
         <v>42</v>
       </c>
-      <c r="B4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>43</v>
-      </c>
-      <c r="E4" t="s">
-        <v>44</v>
       </c>
       <c r="K4">
         <v>100</v>
@@ -1268,10 +1274,10 @@
       <c r="AL4" s="3"/>
       <c r="AM4" s="3"/>
       <c r="AN4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AO4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AP4" s="5">
         <v>0</v>
@@ -1280,19 +1286,19 @@
     </row>
     <row r="5" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" t="s">
         <v>45</v>
       </c>
-      <c r="B5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>46</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>47</v>
-      </c>
-      <c r="E5" t="s">
-        <v>48</v>
       </c>
       <c r="H5">
         <v>52</v>
@@ -1311,16 +1317,16 @@
         <v>0.1</v>
       </c>
       <c r="AL5" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AM5" s="4">
         <v>20.192799999999998</v>
       </c>
       <c r="AN5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AO5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AP5" s="5">
         <v>0</v>
@@ -1329,22 +1335,22 @@
     </row>
     <row r="6" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" t="s">
         <v>40</v>
-      </c>
-      <c r="D6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F6" t="s">
-        <v>41</v>
       </c>
       <c r="K6">
         <v>52</v>
@@ -1359,7 +1365,7 @@
         <v>0.7</v>
       </c>
       <c r="P6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q6">
         <v>0.5</v>
@@ -1392,10 +1398,10 @@
       <c r="AL6" s="3"/>
       <c r="AM6" s="3"/>
       <c r="AN6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AO6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AP6" s="5">
         <v>0</v>
@@ -1404,19 +1410,19 @@
     </row>
     <row r="7" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G7">
         <v>100</v>
@@ -1439,23 +1445,43 @@
       <c r="AL7" s="3"/>
       <c r="AM7" s="3"/>
       <c r="AN7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AO7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AP7" s="5">
         <v>0</v>
       </c>
       <c r="AQ7" s="2"/>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.35">
-      <c r="C9" s="1"/>
+    <row r="8" spans="1:43" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B8" t="s">
+        <v>111</v>
+      </c>
+      <c r="E8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL8" s="3"/>
+      <c r="AM8" s="3"/>
+      <c r="AN8" t="s">
+        <v>92</v>
+      </c>
+      <c r="AO8" t="s">
+        <v>101</v>
+      </c>
+      <c r="AP8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ8" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL2:AL7" xr:uid="{D92CB468-B7A9-4082-9B81-D3B4634F286E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL2:AL8" xr:uid="{D92CB468-B7A9-4082-9B81-D3B4634F286E}">
       <formula1>"h, D, W, M, Q, Y"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1484,7 +1510,7 @@
   <dimension ref="A1:AB5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AB7" sqref="AB7"/>
+      <selection activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1516,10 +1542,10 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1534,7 +1560,7 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
@@ -1552,7 +1578,7 @@
         <v>9</v>
       </c>
       <c r="M1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N1" t="s">
         <v>11</v>
@@ -1561,7 +1587,7 @@
         <v>12</v>
       </c>
       <c r="P1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q1" t="s">
         <v>23</v>
@@ -1573,7 +1599,7 @@
         <v>25</v>
       </c>
       <c r="T1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="U1" t="s">
         <v>26</v>
@@ -1594,33 +1620,33 @@
         <v>32</v>
       </c>
       <c r="AA1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB1" t="s">
         <v>88</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" t="s">
         <v>57</v>
       </c>
-      <c r="B2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" t="s">
         <v>58</v>
-      </c>
-      <c r="D2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G2" t="s">
-        <v>59</v>
       </c>
       <c r="H2">
         <v>1000</v>
@@ -1653,7 +1679,7 @@
         <v>1</v>
       </c>
       <c r="AA2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AB2">
         <v>1</v>
@@ -1661,25 +1687,25 @@
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s">
         <v>60</v>
       </c>
-      <c r="B3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" t="s">
-        <v>61</v>
-      </c>
       <c r="E3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H3">
         <v>1000</v>
@@ -1709,7 +1735,7 @@
         <v>7.2835616438356163E-2</v>
       </c>
       <c r="AA3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AB3">
         <v>1</v>
@@ -1717,25 +1743,25 @@
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" t="s">
         <v>62</v>
       </c>
-      <c r="B4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" t="s">
-        <v>63</v>
-      </c>
       <c r="E4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H4">
         <v>1000</v>
@@ -1765,7 +1791,7 @@
         <v>1.0958904109589041E-2</v>
       </c>
       <c r="AA4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AB4">
         <v>1</v>
@@ -1773,19 +1799,19 @@
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" t="s">
         <v>64</v>
       </c>
-      <c r="B5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>65</v>
-      </c>
-      <c r="G5" t="s">
-        <v>66</v>
       </c>
       <c r="H5">
         <v>1000</v>
@@ -1803,7 +1829,7 @@
         <v>1</v>
       </c>
       <c r="AA5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AB5">
         <v>1</v>
@@ -1857,28 +1883,28 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" t="s">
         <v>67</v>
       </c>
-      <c r="B1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>68</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>69</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>70</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>71</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>72</v>
-      </c>
-      <c r="H1" t="s">
-        <v>73</v>
       </c>
       <c r="I1" t="s">
         <v>26</v>
@@ -1890,21 +1916,21 @@
         <v>28</v>
       </c>
       <c r="L1" t="s">
+        <v>84</v>
+      </c>
+      <c r="M1" t="s">
         <v>85</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>86</v>
-      </c>
-      <c r="N1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1919,10 +1945,10 @@
         <v>4.147E-2</v>
       </c>
       <c r="H2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -1933,10 +1959,10 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1951,10 +1977,10 @@
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -1991,10 +2017,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71DC79B9-9C58-497E-9FD8-D3F2239E9BDC}">
-  <dimension ref="A1:A16"/>
+  <dimension ref="A1:A17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2004,82 +2030,87 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>109</v>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added start_up/shut_down costs, fixed wind availability onshore/offshore, expanded investment into wind onshore/offshore
Everything is now only created when it is absolutely needed to avoid unnecessary build up time for the model.
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base_methanol.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base_methanol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/methanol/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="146" documentId="13_ncr:1_{D954787A-120F-4E9B-9D31-96F6A5AD2E25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67381982-FD47-4702-BDBD-A0A026002BDB}"/>
+  <xr:revisionPtr revIDLastSave="183" documentId="13_ncr:1_{D954787A-120F-4E9B-9D31-96F6A5AD2E25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6623D91-A59E-40B2-8FB1-AA7C413DA206}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="Drop_Down" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="CIQWBGuid" hidden="1">"05b51968-c522-4eae-92ba-f2b2408101af"</definedName>
+    <definedName name="CIQWBGuid" hidden="1">"378badc6-b550-4849-a0fc-5509a5582dd3"</definedName>
     <definedName name="CIQWBInfo" hidden="1">"{ ""CIQVersion"":""9.51.3510.3078"" }"</definedName>
     <definedName name="IQ_CH">110000</definedName>
     <definedName name="IQ_CQ">5000</definedName>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="105">
   <si>
     <t>Unit</t>
   </si>
@@ -382,6 +382,12 @@
   </si>
   <si>
     <t>Wind_offshore</t>
+  </si>
+  <si>
+    <t>start_up_cost</t>
+  </si>
+  <si>
+    <t>shut_down_cost</t>
   </si>
 </sst>
 </file>
@@ -527,9 +533,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:AN7" totalsRowShown="0">
-  <autoFilter ref="A1:AN7" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
-  <tableColumns count="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:AP7" totalsRowShown="0">
+  <autoFilter ref="A1:AP7" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
+  <tableColumns count="42">
     <tableColumn id="1" xr3:uid="{C73E51D0-1842-42F3-9C00-F0DBD2E661BE}" name="Unit"/>
     <tableColumn id="40" xr3:uid="{C2CFC5A4-5329-4F74-926A-18CEB18C062C}" name="Object_type"/>
     <tableColumn id="2" xr3:uid="{FA8BE796-DE15-407E-8998-92C973AE35A4}" name="Input1"/>
@@ -554,6 +560,8 @@
     <tableColumn id="31" xr3:uid="{FF26E17F-A633-477F-A8B8-3FD0C0B88F7D}" name="start_up_Output2"/>
     <tableColumn id="32" xr3:uid="{D45EEC70-4FBC-44FF-9E9A-E2D38C52BF94}" name="shut_down_Output1"/>
     <tableColumn id="33" xr3:uid="{D8C88D78-E68F-45EF-8A97-7C1F84821946}" name="shut_down_Output2"/>
+    <tableColumn id="36" xr3:uid="{1EE4296C-1C46-4898-8A2C-751BA3F253FD}" name="start_up_cost"/>
+    <tableColumn id="37" xr3:uid="{6C1B7D2C-C9EA-4CA7-8F83-97D715B96047}" name="shut_down_cost"/>
     <tableColumn id="9" xr3:uid="{50F936EF-D32C-4938-8FCA-291A6A3E82E6}" name="Relation_In_In"/>
     <tableColumn id="20" xr3:uid="{84C680FD-12EA-4AE2-A238-57453A3D8C12}" name="Relation_In_Out"/>
     <tableColumn id="10" xr3:uid="{ACDE4024-BCA2-4145-B3BC-1A5A08F3EA7D}" name="Relation_Out_Out"/>
@@ -942,10 +950,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
-  <dimension ref="A1:AN7"/>
+  <dimension ref="A1:AP7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AH12" sqref="AH12"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y8" sqref="Y8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -962,21 +970,21 @@
     <col min="13" max="13" width="21.81640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="19" customWidth="1"/>
     <col min="15" max="15" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="16" max="24" width="10.54296875" customWidth="1"/>
-    <col min="25" max="25" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="12.7265625" customWidth="1"/>
-    <col min="30" max="30" width="11" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11" customWidth="1"/>
-    <col min="32" max="32" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="8.7265625" customWidth="1"/>
-    <col min="37" max="37" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="10" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="17.36328125" customWidth="1"/>
+    <col min="16" max="26" width="10.54296875" customWidth="1"/>
+    <col min="27" max="27" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="12.7265625" customWidth="1"/>
+    <col min="32" max="32" width="11" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11" customWidth="1"/>
+    <col min="34" max="34" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="8.7265625" customWidth="1"/>
+    <col min="39" max="39" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="10" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="17.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1050,55 +1058,61 @@
         <v>22</v>
       </c>
       <c r="Y1" t="s">
+        <v>103</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>93</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>27</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AG1" t="s">
         <v>28</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AH1" t="s">
         <v>29</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AI1" t="s">
         <v>30</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AJ1" t="s">
         <v>31</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AK1" t="s">
         <v>32</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AL1" t="s">
         <v>33</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AM1" t="s">
         <v>73</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AN1" t="s">
         <v>74</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AO1" t="s">
         <v>87</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>100</v>
       </c>
@@ -1114,21 +1128,24 @@
       <c r="L2">
         <v>304</v>
       </c>
-      <c r="AB2">
+      <c r="Y2">
+        <v>10</v>
+      </c>
+      <c r="AD2">
         <f>Table1[[#This Row],[Cap_Output1_existing]]*0.56</f>
         <v>170.24</v>
       </c>
-      <c r="AD2">
+      <c r="AF2">
         <v>1.29</v>
       </c>
-      <c r="AK2" s="3"/>
-      <c r="AL2" s="3"/>
-      <c r="AM2" s="5">
+      <c r="AM2" s="3"/>
+      <c r="AN2" s="3"/>
+      <c r="AO2" s="5">
         <v>0</v>
       </c>
-      <c r="AN2" s="2"/>
-    </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="AP2" s="2"/>
+    </row>
+    <row r="3" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -1156,29 +1173,29 @@
       <c r="O3">
         <v>0.75</v>
       </c>
-      <c r="Y3">
+      <c r="AA3">
         <v>5.8500000000000002E-3</v>
       </c>
-      <c r="AA3">
+      <c r="AC3">
         <v>1.76</v>
       </c>
-      <c r="AD3">
+      <c r="AF3">
         <v>4.34</v>
       </c>
-      <c r="AG3">
+      <c r="AI3">
         <v>1.4865951742627345E-3</v>
       </c>
-      <c r="AJ3">
+      <c r="AL3">
         <v>0.02</v>
       </c>
-      <c r="AK3" s="3"/>
-      <c r="AL3" s="3"/>
-      <c r="AM3" s="5">
+      <c r="AM3" s="3"/>
+      <c r="AN3" s="3"/>
+      <c r="AO3" s="5">
         <v>0</v>
       </c>
-      <c r="AN3" s="2"/>
-    </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="AP3" s="2"/>
+    </row>
+    <row r="4" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -1200,23 +1217,23 @@
       <c r="L4">
         <v>100</v>
       </c>
-      <c r="Y4">
+      <c r="AA4">
         <v>3.6010731197896975E-3</v>
       </c>
-      <c r="Z4">
+      <c r="AB4">
         <v>3.601073119789697E-3</v>
       </c>
-      <c r="AF4">
+      <c r="AH4">
         <v>26.81</v>
       </c>
-      <c r="AK4" s="3"/>
-      <c r="AL4" s="3"/>
-      <c r="AM4" s="5">
+      <c r="AM4" s="3"/>
+      <c r="AN4" s="3"/>
+      <c r="AO4" s="5">
         <v>0</v>
       </c>
-      <c r="AN4" s="2"/>
-    </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="AP4" s="2"/>
+    </row>
+    <row r="5" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -1238,25 +1255,25 @@
       <c r="K5">
         <v>52</v>
       </c>
-      <c r="Y5">
+      <c r="AA5">
         <v>17.277901743828668</v>
       </c>
-      <c r="Z5">
+      <c r="AB5">
         <f>1/0.795</f>
         <v>1.2578616352201257</v>
       </c>
-      <c r="AK5" s="3" t="s">
+      <c r="AM5" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="AL5" s="4">
+      <c r="AN5" s="4">
         <v>20.192799999999998</v>
       </c>
-      <c r="AM5" s="5">
+      <c r="AO5" s="5">
         <v>0</v>
       </c>
-      <c r="AN5" s="2"/>
-    </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="AP5" s="2"/>
+    </row>
+    <row r="6" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -1302,27 +1319,27 @@
       <c r="W6">
         <v>0.5</v>
       </c>
-      <c r="Y6">
+      <c r="AA6">
         <v>5.1734967222388608</v>
       </c>
-      <c r="Z6">
+      <c r="AB6">
         <f>1/0.96</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="AA6">
+      <c r="AC6">
         <v>4.32</v>
       </c>
-      <c r="AD6">
+      <c r="AF6">
         <v>4.45</v>
       </c>
-      <c r="AK6" s="3"/>
-      <c r="AL6" s="3"/>
-      <c r="AM6" s="5">
+      <c r="AM6" s="3"/>
+      <c r="AN6" s="3"/>
+      <c r="AO6" s="5">
         <v>0</v>
       </c>
-      <c r="AN6" s="2"/>
-    </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="AP6" s="2"/>
+    </row>
+    <row r="7" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -1341,29 +1358,29 @@
       <c r="G7">
         <v>100</v>
       </c>
-      <c r="Y7">
+      <c r="AA7">
         <v>7.2437800000000002E-4</v>
       </c>
-      <c r="Z7">
+      <c r="AB7">
         <v>0.99</v>
       </c>
-      <c r="AD7">
+      <c r="AF7">
         <v>0.11929223744292237</v>
       </c>
-      <c r="AG7">
+      <c r="AI7">
         <v>1.4865951742627345E-3</v>
       </c>
-      <c r="AK7" s="3"/>
-      <c r="AL7" s="3"/>
-      <c r="AM7" s="5">
+      <c r="AM7" s="3"/>
+      <c r="AN7" s="3"/>
+      <c r="AO7" s="5">
         <v>0</v>
       </c>
-      <c r="AN7" s="2"/>
+      <c r="AP7" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK2:AK7" xr:uid="{D92CB468-B7A9-4082-9B81-D3B4634F286E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2:AM7" xr:uid="{D92CB468-B7A9-4082-9B81-D3B4634F286E}">
       <formula1>"h, D, W, M, Q, Y"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
remove pv start up costs from input data
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base_methanol.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base_methanol.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/methanol/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="183" documentId="13_ncr:1_{D954787A-120F-4E9B-9D31-96F6A5AD2E25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6623D91-A59E-40B2-8FB1-AA7C413DA206}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A6B789D-D89E-4749-B72E-CE41F125F646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-2790" yWindow="-19440" windowWidth="28800" windowHeight="15225" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -952,8 +952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:AP7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y8" sqref="Y8"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y3" sqref="Y3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1127,9 +1127,6 @@
       </c>
       <c r="L2">
         <v>304</v>
-      </c>
-      <c r="Y2">
-        <v>10</v>
       </c>
       <c r="AD2">
         <f>Table1[[#This Row],[Cap_Output1_existing]]*0.56</f>

</xml_diff>

<commit_message>
Set capacity limits in node data frame and adjusted mapping
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base_methanol.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base_methanol.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/luc_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/methanol/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A6B789D-D89E-4749-B72E-CE41F125F646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{1A6B789D-D89E-4749-B72E-CE41F125F646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C2D96BBF-E936-4A1B-983B-1FB5C7C31686}"/>
   <bookViews>
-    <workbookView xWindow="-2790" yWindow="-19440" windowWidth="28800" windowHeight="15225" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -952,7 +952,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:AP7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="Y3" sqref="Y3"/>
     </sheetView>
   </sheetViews>
@@ -1405,8 +1405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C870BDA0-9E4C-481D-87BE-9D47789809C8}">
   <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S7" sqref="S7"/>
+    <sheetView topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1753,7 +1753,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{981CFA5E-60F3-446F-A856-2FA65B76879A}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -1770,6 +1770,8 @@
     <col min="9" max="9" width="9" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.1796875" customWidth="1"/>
+    <col min="13" max="13" width="24.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
fix initial units and investment limit bug
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base_methanol.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base_methanol.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/luc_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/methanol/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{1A6B789D-D89E-4749-B72E-CE41F125F646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C2D96BBF-E936-4A1B-983B-1FB5C7C31686}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24396502-44B5-42C2-B74E-8B271D2632C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -324,21 +324,12 @@
     <t>Hydrogen_storage</t>
   </si>
   <si>
-    <t>number_of_storages</t>
-  </si>
-  <si>
     <t>storage_investment_cost</t>
   </si>
   <si>
     <t>connection_investment_tech_lifetime</t>
   </si>
   <si>
-    <t>number_of_connections</t>
-  </si>
-  <si>
-    <t>number_of_units</t>
-  </si>
-  <si>
     <t>Pipeline</t>
   </si>
   <si>
@@ -388,6 +379,15 @@
   </si>
   <si>
     <t>shut_down_cost</t>
+  </si>
+  <si>
+    <t>initial_units_invested_available</t>
+  </si>
+  <si>
+    <t>initial_connections_invested_available</t>
+  </si>
+  <si>
+    <t>initial_storages_invested</t>
   </si>
 </sst>
 </file>
@@ -576,7 +576,7 @@
     <tableColumn id="34" xr3:uid="{7D7F0E89-0553-40E4-9D5A-219BF1741787}" name="minimum_op_point"/>
     <tableColumn id="38" xr3:uid="{957AF85B-8792-4643-A381-29FACAA69887}" name="resolution_output" dataDxfId="6"/>
     <tableColumn id="39" xr3:uid="{BCE2350E-150B-4A7E-94BF-BB3BC7E31016}" name="demand" dataDxfId="5"/>
-    <tableColumn id="43" xr3:uid="{4079FBE2-CFC5-4BCF-9353-8F6771C73DD2}" name="number_of_units" dataDxfId="4"/>
+    <tableColumn id="43" xr3:uid="{4079FBE2-CFC5-4BCF-9353-8F6771C73DD2}" name="initial_units_invested_available" dataDxfId="4"/>
     <tableColumn id="45" xr3:uid="{4B3B8871-E458-49D5-BFE4-E2DD849EE6AD}" name="Error messages:" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -613,7 +613,7 @@
     <tableColumn id="24" xr3:uid="{41B338E4-2058-41E9-8000-97D77450FBC3}" name="vom_cost_Output1"/>
     <tableColumn id="25" xr3:uid="{DDAFCF0A-1EF1-4B7B-9742-01F9FA7A22E5}" name="vom_cost_Output2"/>
     <tableColumn id="29" xr3:uid="{79DE3A19-CED6-47DE-AEF5-F6BB2D320F24}" name="connection_investment_tech_lifetime" dataDxfId="1"/>
-    <tableColumn id="30" xr3:uid="{09434E4A-7BF5-4547-9708-EA3F0F7ADC8E}" name="number_of_connections"/>
+    <tableColumn id="30" xr3:uid="{09434E4A-7BF5-4547-9708-EA3F0F7ADC8E}" name="initial_connections_invested_available"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -636,7 +636,7 @@
     <tableColumn id="11" xr3:uid="{3C880482-B284-4120-859D-C69724716B06}" name="Cost_invest"/>
     <tableColumn id="12" xr3:uid="{DC155748-1945-4E24-B8A1-527B52E12445}" name="fom_cost"/>
     <tableColumn id="13" xr3:uid="{620A5657-4B04-4066-87F7-215E607C4C88}" name="vom_cost"/>
-    <tableColumn id="15" xr3:uid="{5FF71707-8528-4768-8697-8818F4BC14D6}" name="number_of_storages"/>
+    <tableColumn id="15" xr3:uid="{5FF71707-8528-4768-8697-8818F4BC14D6}" name="initial_storages_invested"/>
     <tableColumn id="16" xr3:uid="{8C607D2E-BC5C-4E67-8BF2-33EAD803CDBB}" name="storage_investment_cost"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -952,8 +952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:AP7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y3" sqref="Y3"/>
+    <sheetView topLeftCell="AC1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AO2" sqref="AO2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1058,10 +1058,10 @@
         <v>22</v>
       </c>
       <c r="Y1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="Z1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="AA1" t="s">
         <v>23</v>
@@ -1076,7 +1076,7 @@
         <v>26</v>
       </c>
       <c r="AE1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="AF1" t="s">
         <v>27</v>
@@ -1106,7 +1106,7 @@
         <v>74</v>
       </c>
       <c r="AO1" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="AP1" s="1" t="s">
         <v>34</v>
@@ -1114,7 +1114,7 @@
     </row>
     <row r="2" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
         <v>77</v>
@@ -1147,7 +1147,7 @@
         <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C3" t="s">
         <v>35</v>
@@ -1235,7 +1235,7 @@
         <v>43</v>
       </c>
       <c r="B5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C5" t="s">
         <v>44</v>
@@ -1405,8 +1405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C870BDA0-9E4C-481D-87BE-9D47789809C8}">
   <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1512,10 +1512,10 @@
         <v>32</v>
       </c>
       <c r="Z1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AA1" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.35">
@@ -1523,7 +1523,7 @@
         <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C2" t="s">
         <v>56</v>
@@ -1571,7 +1571,7 @@
         <v>1</v>
       </c>
       <c r="Z2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="AA2">
         <v>1</v>
@@ -1582,7 +1582,7 @@
         <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C3" t="s">
         <v>38</v>
@@ -1627,7 +1627,7 @@
         <v>7.2835616438356163E-2</v>
       </c>
       <c r="Z3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="AA3">
         <v>1</v>
@@ -1638,7 +1638,7 @@
         <v>60</v>
       </c>
       <c r="B4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C4" t="s">
         <v>46</v>
@@ -1683,7 +1683,7 @@
         <v>1.0958904109589041E-2</v>
       </c>
       <c r="Z4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="AA4">
         <v>1</v>
@@ -1694,7 +1694,7 @@
         <v>62</v>
       </c>
       <c r="B5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C5" t="s">
         <v>39</v>
@@ -1721,7 +1721,7 @@
         <v>1</v>
       </c>
       <c r="Z5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="AA5">
         <v>1</v>
@@ -1753,8 +1753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{981CFA5E-60F3-446F-A856-2FA65B76879A}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1809,10 +1809,10 @@
         <v>28</v>
       </c>
       <c r="L1" t="s">
+        <v>104</v>
+      </c>
+      <c r="M1" t="s">
         <v>83</v>
-      </c>
-      <c r="M1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
@@ -1904,7 +1904,7 @@
   <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1924,17 +1924,17 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
@@ -1964,42 +1964,42 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Comprehensive update to remove capacities from table
Now only capacities from main dropdowns are used.
Careful to always choose the right capacities for our project - could be worth it to change the defaults for the duration of our project
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base_methanol.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base_methanol.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/methanol/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24396502-44B5-42C2-B74E-8B271D2632C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{24396502-44B5-42C2-B74E-8B271D2632C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AFE21F23-F208-404E-944F-D34D3585F9E6}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Drop_Down" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="CIQWBGuid" hidden="1">"378badc6-b550-4849-a0fc-5509a5582dd3"</definedName>
+    <definedName name="CIQWBGuid" hidden="1">"3701cb1e-3b63-4ab2-a684-fdb01043e14d"</definedName>
     <definedName name="CIQWBInfo" hidden="1">"{ ""CIQVersion"":""9.51.3510.3078"" }"</definedName>
     <definedName name="IQ_CH">110000</definedName>
     <definedName name="IQ_CQ">5000</definedName>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="104">
   <si>
     <t>Unit</t>
   </si>
@@ -103,9 +103,6 @@
   </si>
   <si>
     <t>Cap_Output1_existing</t>
-  </si>
-  <si>
-    <t>Cap_Output_1_max</t>
   </si>
   <si>
     <t>Cap_Output2_existing</t>
@@ -533,23 +530,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:AP7" totalsRowShown="0">
-  <autoFilter ref="A1:AP7" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
-  <tableColumns count="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:AH7" totalsRowShown="0">
+  <autoFilter ref="A1:AH7" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
+  <tableColumns count="34">
     <tableColumn id="1" xr3:uid="{C73E51D0-1842-42F3-9C00-F0DBD2E661BE}" name="Unit"/>
     <tableColumn id="40" xr3:uid="{C2CFC5A4-5329-4F74-926A-18CEB18C062C}" name="Object_type"/>
     <tableColumn id="2" xr3:uid="{FA8BE796-DE15-407E-8998-92C973AE35A4}" name="Input1"/>
     <tableColumn id="3" xr3:uid="{168877A6-E181-4446-9569-F36E8CEB8908}" name="Input2"/>
     <tableColumn id="4" xr3:uid="{C03E717E-B39B-450F-A07B-8C087AA65297}" name="Output1"/>
     <tableColumn id="5" xr3:uid="{1193D369-BC65-45A6-8749-4CD88E2C1722}" name="Output2"/>
-    <tableColumn id="6" xr3:uid="{4AAC878F-692F-4277-A013-661DCC5DAE26}" name="Cap_Input1_existing"/>
-    <tableColumn id="7" xr3:uid="{C21757F9-61E8-45D7-ADA3-80D8624CAEF0}" name="Cap_Input1_max"/>
-    <tableColumn id="14" xr3:uid="{23796EE3-B67D-45AE-9553-CC3081EFDF57}" name="Cap_Input2_existing"/>
-    <tableColumn id="15" xr3:uid="{DF0C0799-CA68-4E9B-A1FB-41F4996C01A9}" name="Cap_Input2_max"/>
-    <tableColumn id="16" xr3:uid="{8A84DF9A-0F8E-4DA8-A009-F41EF2B05A60}" name="Cap_Output1_existing"/>
-    <tableColumn id="17" xr3:uid="{6408F114-841E-472E-92F5-7B63FF1B66F4}" name="Cap_Output_1_max"/>
-    <tableColumn id="18" xr3:uid="{541C17F0-C020-47FE-9DA4-DB76D7416668}" name="Cap_Output2_existing"/>
-    <tableColumn id="19" xr3:uid="{D6FEE63D-DC89-4D1A-9708-5E7C70FD5793}" name="Cap_Output2_max"/>
     <tableColumn id="35" xr3:uid="{C3887B4E-C4A5-42AB-A92F-97AD44212E95}" name="mean_efficiency"/>
     <tableColumn id="8" xr3:uid="{5F719CEE-A0F7-452C-B82C-E739C5FED49B}" name="min_down_time"/>
     <tableColumn id="26" xr3:uid="{D0F85E7B-D704-45A0-BE99-26E3A1F08634}" name="ramp_up_Output1"/>
@@ -950,10 +939,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
-  <dimension ref="A1:AP7"/>
+  <dimension ref="A1:AH7"/>
   <sheetViews>
-    <sheetView topLeftCell="AC1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AO2" sqref="AO2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -961,35 +950,27 @@
     <col min="1" max="1" width="13.81640625" customWidth="1"/>
     <col min="2" max="2" width="19.36328125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9.81640625" customWidth="1"/>
-    <col min="7" max="7" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.453125" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.453125" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="21.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.1796875" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="21.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19" customWidth="1"/>
-    <col min="15" max="15" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="16" max="26" width="10.54296875" customWidth="1"/>
-    <col min="27" max="27" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="12.7265625" customWidth="1"/>
-    <col min="32" max="32" width="11" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11" customWidth="1"/>
-    <col min="34" max="34" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="8.7265625" customWidth="1"/>
-    <col min="39" max="39" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="10" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="17.36328125" customWidth="1"/>
+    <col min="7" max="7" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="18" width="10.54296875" customWidth="1"/>
+    <col min="19" max="19" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="12.7265625" customWidth="1"/>
+    <col min="24" max="24" width="11" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11" customWidth="1"/>
+    <col min="26" max="26" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.7265625" customWidth="1"/>
+    <col min="31" max="31" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="17.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1004,380 +985,320 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="J1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="L1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="M1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="N1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="O1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="P1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="Q1" t="s">
-        <v>15</v>
+        <v>99</v>
       </c>
       <c r="R1" t="s">
-        <v>16</v>
+        <v>100</v>
       </c>
       <c r="S1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="T1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="U1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="V1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="W1" t="s">
-        <v>21</v>
+        <v>89</v>
       </c>
       <c r="X1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="Y1" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="Z1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AG1" t="s">
         <v>101</v>
       </c>
-      <c r="AA1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AL1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AM1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>102</v>
-      </c>
-      <c r="AP1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="V2" t="e">
+        <f>#REF!*0.56</f>
+        <v>#REF!</v>
+      </c>
+      <c r="X2">
+        <v>1.29</v>
+      </c>
+      <c r="AE2" s="3"/>
+      <c r="AF2" s="3"/>
+      <c r="AG2" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="2"/>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>35</v>
       </c>
-      <c r="K2">
-        <v>304</v>
-      </c>
-      <c r="L2">
-        <v>304</v>
-      </c>
-      <c r="AD2">
-        <f>Table1[[#This Row],[Cap_Output1_existing]]*0.56</f>
-        <v>170.24</v>
-      </c>
-      <c r="AF2">
-        <v>1.29</v>
-      </c>
-      <c r="AM2" s="3"/>
-      <c r="AN2" s="3"/>
-      <c r="AO2" s="5">
+      <c r="B3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3">
+        <v>0.75</v>
+      </c>
+      <c r="S3">
+        <v>5.8500000000000002E-3</v>
+      </c>
+      <c r="U3">
+        <v>1.76</v>
+      </c>
+      <c r="X3">
+        <v>4.34</v>
+      </c>
+      <c r="AA3">
+        <v>1.4865951742627345E-3</v>
+      </c>
+      <c r="AD3">
+        <v>0.02</v>
+      </c>
+      <c r="AE3" s="3"/>
+      <c r="AF3" s="3"/>
+      <c r="AG3" s="5">
         <v>0</v>
       </c>
-      <c r="AP2" s="2"/>
-    </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="AH3" s="2"/>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>39</v>
       </c>
-      <c r="G3">
-        <v>52</v>
-      </c>
-      <c r="H3">
-        <v>52</v>
-      </c>
-      <c r="O3">
-        <v>0.75</v>
-      </c>
-      <c r="AA3">
-        <v>5.8500000000000002E-3</v>
-      </c>
-      <c r="AC3">
-        <v>1.76</v>
-      </c>
-      <c r="AF3">
-        <v>4.34</v>
-      </c>
-      <c r="AI3">
-        <v>1.4865951742627345E-3</v>
-      </c>
-      <c r="AL3">
-        <v>0.02</v>
-      </c>
-      <c r="AM3" s="3"/>
-      <c r="AN3" s="3"/>
-      <c r="AO3" s="5">
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" t="s">
+        <v>41</v>
+      </c>
+      <c r="S4">
+        <v>3.6010731197896975E-3</v>
+      </c>
+      <c r="T4">
+        <v>3.601073119789697E-3</v>
+      </c>
+      <c r="Z4">
+        <v>26.81</v>
+      </c>
+      <c r="AE4" s="3"/>
+      <c r="AF4" s="3"/>
+      <c r="AG4" s="5">
         <v>0</v>
       </c>
-      <c r="AP3" s="2"/>
-    </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="AH4" s="2"/>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>42</v>
       </c>
-      <c r="K4">
-        <v>100</v>
-      </c>
-      <c r="L4">
-        <v>100</v>
-      </c>
-      <c r="AA4">
-        <v>3.6010731197896975E-3</v>
-      </c>
-      <c r="AB4">
-        <v>3.601073119789697E-3</v>
-      </c>
-      <c r="AH4">
-        <v>26.81</v>
-      </c>
-      <c r="AM4" s="3"/>
-      <c r="AN4" s="3"/>
-      <c r="AO4" s="5">
-        <v>0</v>
-      </c>
-      <c r="AP4" s="2"/>
-    </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" t="s">
         <v>43</v>
       </c>
-      <c r="B5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>44</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>45</v>
       </c>
-      <c r="E5" t="s">
-        <v>46</v>
-      </c>
-      <c r="H5">
-        <v>52</v>
-      </c>
-      <c r="K5">
-        <v>52</v>
-      </c>
-      <c r="AA5">
+      <c r="S5">
         <v>17.277901743828668</v>
       </c>
-      <c r="AB5">
+      <c r="T5">
         <f>1/0.795</f>
         <v>1.2578616352201257</v>
       </c>
-      <c r="AM5" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="AN5" s="4">
+      <c r="AE5" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AF5" s="4">
         <v>20.192799999999998</v>
       </c>
-      <c r="AO5" s="5">
+      <c r="AG5" s="5">
         <v>0</v>
       </c>
-      <c r="AP5" s="2"/>
-    </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="AH5" s="2"/>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6">
+        <v>0.7</v>
+      </c>
+      <c r="H6" t="s">
         <v>47</v>
       </c>
-      <c r="B6" t="s">
-        <v>80</v>
-      </c>
-      <c r="C6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F6" t="s">
-        <v>39</v>
+      <c r="I6">
+        <v>0.5</v>
       </c>
       <c r="K6">
-        <v>52</v>
-      </c>
-      <c r="L6">
-        <v>100</v>
-      </c>
-      <c r="N6">
-        <v>10</v>
+        <v>0.5</v>
+      </c>
+      <c r="M6">
+        <v>0.5</v>
       </c>
       <c r="O6">
-        <v>0.7</v>
-      </c>
-      <c r="P6" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q6">
         <v>0.5</v>
       </c>
       <c r="S6">
-        <v>0.5</v>
-      </c>
-      <c r="U6">
-        <v>0.5</v>
-      </c>
-      <c r="W6">
-        <v>0.5</v>
-      </c>
-      <c r="AA6">
         <v>5.1734967222388608</v>
       </c>
-      <c r="AB6">
+      <c r="T6">
         <f>1/0.96</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="AC6">
+      <c r="U6">
         <v>4.32</v>
       </c>
-      <c r="AF6">
+      <c r="X6">
         <v>4.45</v>
       </c>
-      <c r="AM6" s="3"/>
-      <c r="AN6" s="3"/>
-      <c r="AO6" s="5">
+      <c r="AE6" s="3"/>
+      <c r="AF6" s="3"/>
+      <c r="AG6" s="5">
         <v>0</v>
       </c>
-      <c r="AP6" s="2"/>
-    </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="AH6" s="2"/>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G7">
-        <v>100</v>
+        <v>44</v>
+      </c>
+      <c r="S7">
+        <v>7.2437800000000002E-4</v>
+      </c>
+      <c r="T7">
+        <v>0.99</v>
+      </c>
+      <c r="X7">
+        <v>0.11929223744292237</v>
       </c>
       <c r="AA7">
-        <v>7.2437800000000002E-4</v>
-      </c>
-      <c r="AB7">
-        <v>0.99</v>
-      </c>
-      <c r="AF7">
-        <v>0.11929223744292237</v>
-      </c>
-      <c r="AI7">
         <v>1.4865951742627345E-3</v>
       </c>
-      <c r="AM7" s="3"/>
-      <c r="AN7" s="3"/>
-      <c r="AO7" s="5">
+      <c r="AE7" s="3"/>
+      <c r="AF7" s="3"/>
+      <c r="AG7" s="5">
         <v>0</v>
       </c>
-      <c r="AP7" s="2"/>
+      <c r="AH7" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2:AM7" xr:uid="{D92CB468-B7A9-4082-9B81-D3B4634F286E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE2:AE7" xr:uid="{D92CB468-B7A9-4082-9B81-D3B4634F286E}">
       <formula1>"h, D, W, M, Q, Y"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1437,10 +1358,10 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1455,7 +1376,7 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
@@ -1473,72 +1394,72 @@
         <v>9</v>
       </c>
       <c r="M1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" t="s">
         <v>52</v>
       </c>
-      <c r="N1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" t="s">
         <v>53</v>
       </c>
-      <c r="Q1" t="s">
-        <v>23</v>
-      </c>
-      <c r="R1" t="s">
-        <v>24</v>
-      </c>
-      <c r="S1" t="s">
-        <v>25</v>
-      </c>
-      <c r="T1" t="s">
-        <v>54</v>
-      </c>
       <c r="U1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V1" t="s">
+        <v>28</v>
+      </c>
+      <c r="W1" t="s">
         <v>29</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>30</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>31</v>
       </c>
-      <c r="Y1" t="s">
-        <v>32</v>
-      </c>
       <c r="Z1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AA1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" t="s">
         <v>55</v>
       </c>
-      <c r="B2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" t="s">
         <v>56</v>
-      </c>
-      <c r="D2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G2" t="s">
-        <v>57</v>
       </c>
       <c r="H2">
         <v>1000</v>
@@ -1571,7 +1492,7 @@
         <v>1</v>
       </c>
       <c r="Z2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AA2">
         <v>1</v>
@@ -1579,25 +1500,25 @@
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
         <v>58</v>
       </c>
-      <c r="B3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" t="s">
-        <v>59</v>
-      </c>
       <c r="E3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H3">
         <v>1000</v>
@@ -1627,7 +1548,7 @@
         <v>7.2835616438356163E-2</v>
       </c>
       <c r="Z3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA3">
         <v>1</v>
@@ -1635,25 +1556,25 @@
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" t="s">
         <v>60</v>
       </c>
-      <c r="B4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" t="s">
-        <v>61</v>
-      </c>
       <c r="E4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H4">
         <v>1000</v>
@@ -1683,7 +1604,7 @@
         <v>1.0958904109589041E-2</v>
       </c>
       <c r="Z4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA4">
         <v>1</v>
@@ -1691,19 +1612,19 @@
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" t="s">
         <v>62</v>
       </c>
-      <c r="B5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>63</v>
-      </c>
-      <c r="G5" t="s">
-        <v>64</v>
       </c>
       <c r="H5">
         <v>1000</v>
@@ -1721,7 +1642,7 @@
         <v>1</v>
       </c>
       <c r="Z5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AA5">
         <v>1</v>
@@ -1753,7 +1674,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{981CFA5E-60F3-446F-A856-2FA65B76879A}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
@@ -1776,51 +1697,51 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
         <v>65</v>
       </c>
-      <c r="B1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>66</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>67</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>68</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>69</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>70</v>
       </c>
-      <c r="H1" t="s">
-        <v>71</v>
-      </c>
       <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
         <v>26</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>27</v>
       </c>
-      <c r="K1" t="s">
-        <v>28</v>
-      </c>
       <c r="L1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1835,7 +1756,7 @@
         <v>4.147E-2</v>
       </c>
       <c r="H2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -1846,10 +1767,10 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1864,7 +1785,7 @@
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -1914,92 +1835,92 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updte of the co2 vaporizer data
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base_methanol.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base_methanol.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24396502-44B5-42C2-B74E-8B271D2632C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D333C5F-6235-4025-A347-49A5A66A72FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-4590" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -952,8 +952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:AP7"/>
   <sheetViews>
-    <sheetView topLeftCell="AC1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AO2" sqref="AO2"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AE17" sqref="AE17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1215,10 +1215,10 @@
         <v>100</v>
       </c>
       <c r="AA4">
-        <v>3.6010731197896975E-3</v>
+        <v>3.5294117647058825E-3</v>
       </c>
       <c r="AB4">
-        <v>3.601073119789697E-3</v>
+        <v>3.5294117647058825E-3</v>
       </c>
       <c r="AH4">
         <v>26.81</v>
@@ -1753,7 +1753,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{981CFA5E-60F3-446F-A856-2FA65B76879A}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
reintegrate correct data base after merge
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base_methanol.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base_methanol.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D333C5F-6235-4025-A347-49A5A66A72FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2B69A3F-4DB4-48FC-ADEA-E31E281CE886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4590" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Drop_Down" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="CIQWBGuid" hidden="1">"378badc6-b550-4849-a0fc-5509a5582dd3"</definedName>
+    <definedName name="CIQWBGuid" hidden="1">"3701cb1e-3b63-4ab2-a684-fdb01043e14d"</definedName>
     <definedName name="CIQWBInfo" hidden="1">"{ ""CIQVersion"":""9.51.3510.3078"" }"</definedName>
     <definedName name="IQ_CH">110000</definedName>
     <definedName name="IQ_CQ">5000</definedName>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="104">
   <si>
     <t>Unit</t>
   </si>
@@ -103,9 +103,6 @@
   </si>
   <si>
     <t>Cap_Output1_existing</t>
-  </si>
-  <si>
-    <t>Cap_Output_1_max</t>
   </si>
   <si>
     <t>Cap_Output2_existing</t>
@@ -533,23 +530,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:AP7" totalsRowShown="0">
-  <autoFilter ref="A1:AP7" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
-  <tableColumns count="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:AH7" totalsRowShown="0">
+  <autoFilter ref="A1:AH7" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
+  <tableColumns count="34">
     <tableColumn id="1" xr3:uid="{C73E51D0-1842-42F3-9C00-F0DBD2E661BE}" name="Unit"/>
     <tableColumn id="40" xr3:uid="{C2CFC5A4-5329-4F74-926A-18CEB18C062C}" name="Object_type"/>
     <tableColumn id="2" xr3:uid="{FA8BE796-DE15-407E-8998-92C973AE35A4}" name="Input1"/>
     <tableColumn id="3" xr3:uid="{168877A6-E181-4446-9569-F36E8CEB8908}" name="Input2"/>
     <tableColumn id="4" xr3:uid="{C03E717E-B39B-450F-A07B-8C087AA65297}" name="Output1"/>
     <tableColumn id="5" xr3:uid="{1193D369-BC65-45A6-8749-4CD88E2C1722}" name="Output2"/>
-    <tableColumn id="6" xr3:uid="{4AAC878F-692F-4277-A013-661DCC5DAE26}" name="Cap_Input1_existing"/>
-    <tableColumn id="7" xr3:uid="{C21757F9-61E8-45D7-ADA3-80D8624CAEF0}" name="Cap_Input1_max"/>
-    <tableColumn id="14" xr3:uid="{23796EE3-B67D-45AE-9553-CC3081EFDF57}" name="Cap_Input2_existing"/>
-    <tableColumn id="15" xr3:uid="{DF0C0799-CA68-4E9B-A1FB-41F4996C01A9}" name="Cap_Input2_max"/>
-    <tableColumn id="16" xr3:uid="{8A84DF9A-0F8E-4DA8-A009-F41EF2B05A60}" name="Cap_Output1_existing"/>
-    <tableColumn id="17" xr3:uid="{6408F114-841E-472E-92F5-7B63FF1B66F4}" name="Cap_Output_1_max"/>
-    <tableColumn id="18" xr3:uid="{541C17F0-C020-47FE-9DA4-DB76D7416668}" name="Cap_Output2_existing"/>
-    <tableColumn id="19" xr3:uid="{D6FEE63D-DC89-4D1A-9708-5E7C70FD5793}" name="Cap_Output2_max"/>
     <tableColumn id="35" xr3:uid="{C3887B4E-C4A5-42AB-A92F-97AD44212E95}" name="mean_efficiency"/>
     <tableColumn id="8" xr3:uid="{5F719CEE-A0F7-452C-B82C-E739C5FED49B}" name="min_down_time"/>
     <tableColumn id="26" xr3:uid="{D0F85E7B-D704-45A0-BE99-26E3A1F08634}" name="ramp_up_Output1"/>
@@ -950,10 +939,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
-  <dimension ref="A1:AP7"/>
+  <dimension ref="A1:AH7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AE17" sqref="AE17"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -961,35 +950,27 @@
     <col min="1" max="1" width="13.81640625" customWidth="1"/>
     <col min="2" max="2" width="19.36328125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9.81640625" customWidth="1"/>
-    <col min="7" max="7" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.453125" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.453125" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="21.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.1796875" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="21.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19" customWidth="1"/>
-    <col min="15" max="15" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="16" max="26" width="10.54296875" customWidth="1"/>
-    <col min="27" max="27" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="12.7265625" customWidth="1"/>
-    <col min="32" max="32" width="11" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11" customWidth="1"/>
-    <col min="34" max="34" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="8.7265625" customWidth="1"/>
-    <col min="39" max="39" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="10" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="17.36328125" customWidth="1"/>
+    <col min="7" max="7" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="18" width="10.54296875" customWidth="1"/>
+    <col min="19" max="19" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="12.7265625" customWidth="1"/>
+    <col min="24" max="24" width="11" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11" customWidth="1"/>
+    <col min="26" max="26" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.7265625" customWidth="1"/>
+    <col min="31" max="31" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="17.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1004,380 +985,320 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="J1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="L1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="M1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="N1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="O1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="P1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="Q1" t="s">
-        <v>15</v>
+        <v>99</v>
       </c>
       <c r="R1" t="s">
-        <v>16</v>
+        <v>100</v>
       </c>
       <c r="S1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="T1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="U1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="V1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="W1" t="s">
-        <v>21</v>
+        <v>89</v>
       </c>
       <c r="X1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="Y1" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="Z1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AG1" t="s">
         <v>101</v>
       </c>
-      <c r="AA1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AL1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AM1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>102</v>
-      </c>
-      <c r="AP1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="V2" t="e">
+        <f>#REF!*0.56</f>
+        <v>#REF!</v>
+      </c>
+      <c r="X2">
+        <v>1.29</v>
+      </c>
+      <c r="AE2" s="3"/>
+      <c r="AF2" s="3"/>
+      <c r="AG2" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="2"/>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>35</v>
       </c>
-      <c r="K2">
-        <v>304</v>
-      </c>
-      <c r="L2">
-        <v>304</v>
-      </c>
-      <c r="AD2">
-        <f>Table1[[#This Row],[Cap_Output1_existing]]*0.56</f>
-        <v>170.24</v>
-      </c>
-      <c r="AF2">
-        <v>1.29</v>
-      </c>
-      <c r="AM2" s="3"/>
-      <c r="AN2" s="3"/>
-      <c r="AO2" s="5">
+      <c r="B3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3">
+        <v>0.75</v>
+      </c>
+      <c r="S3">
+        <v>5.8500000000000002E-3</v>
+      </c>
+      <c r="U3">
+        <v>1.76</v>
+      </c>
+      <c r="X3">
+        <v>4.34</v>
+      </c>
+      <c r="AA3">
+        <v>1.4865951742627345E-3</v>
+      </c>
+      <c r="AD3">
+        <v>0.02</v>
+      </c>
+      <c r="AE3" s="3"/>
+      <c r="AF3" s="3"/>
+      <c r="AG3" s="5">
         <v>0</v>
       </c>
-      <c r="AP2" s="2"/>
-    </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="AH3" s="2"/>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>39</v>
       </c>
-      <c r="G3">
-        <v>52</v>
-      </c>
-      <c r="H3">
-        <v>52</v>
-      </c>
-      <c r="O3">
-        <v>0.75</v>
-      </c>
-      <c r="AA3">
-        <v>5.8500000000000002E-3</v>
-      </c>
-      <c r="AC3">
-        <v>1.76</v>
-      </c>
-      <c r="AF3">
-        <v>4.34</v>
-      </c>
-      <c r="AI3">
-        <v>1.4865951742627345E-3</v>
-      </c>
-      <c r="AL3">
-        <v>0.02</v>
-      </c>
-      <c r="AM3" s="3"/>
-      <c r="AN3" s="3"/>
-      <c r="AO3" s="5">
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" t="s">
+        <v>41</v>
+      </c>
+      <c r="S4">
+        <v>3.529412E-3</v>
+      </c>
+      <c r="T4">
+        <v>3.529412E-3</v>
+      </c>
+      <c r="Z4">
+        <v>26.81</v>
+      </c>
+      <c r="AE4" s="3"/>
+      <c r="AF4" s="3"/>
+      <c r="AG4" s="5">
         <v>0</v>
       </c>
-      <c r="AP3" s="2"/>
-    </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="AH4" s="2"/>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>42</v>
       </c>
-      <c r="K4">
-        <v>100</v>
-      </c>
-      <c r="L4">
-        <v>100</v>
-      </c>
-      <c r="AA4">
-        <v>3.5294117647058825E-3</v>
-      </c>
-      <c r="AB4">
-        <v>3.5294117647058825E-3</v>
-      </c>
-      <c r="AH4">
-        <v>26.81</v>
-      </c>
-      <c r="AM4" s="3"/>
-      <c r="AN4" s="3"/>
-      <c r="AO4" s="5">
-        <v>0</v>
-      </c>
-      <c r="AP4" s="2"/>
-    </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" t="s">
         <v>43</v>
       </c>
-      <c r="B5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>44</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>45</v>
       </c>
-      <c r="E5" t="s">
-        <v>46</v>
-      </c>
-      <c r="H5">
-        <v>52</v>
-      </c>
-      <c r="K5">
-        <v>52</v>
-      </c>
-      <c r="AA5">
+      <c r="S5">
         <v>17.277901743828668</v>
       </c>
-      <c r="AB5">
+      <c r="T5">
         <f>1/0.795</f>
         <v>1.2578616352201257</v>
       </c>
-      <c r="AM5" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="AN5" s="4">
+      <c r="AE5" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AF5" s="4">
         <v>20.192799999999998</v>
       </c>
-      <c r="AO5" s="5">
+      <c r="AG5" s="5">
         <v>0</v>
       </c>
-      <c r="AP5" s="2"/>
-    </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="AH5" s="2"/>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6">
+        <v>0.7</v>
+      </c>
+      <c r="H6" t="s">
         <v>47</v>
       </c>
-      <c r="B6" t="s">
-        <v>80</v>
-      </c>
-      <c r="C6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F6" t="s">
-        <v>39</v>
+      <c r="I6">
+        <v>0.5</v>
       </c>
       <c r="K6">
-        <v>52</v>
-      </c>
-      <c r="L6">
-        <v>100</v>
-      </c>
-      <c r="N6">
-        <v>10</v>
+        <v>0.5</v>
+      </c>
+      <c r="M6">
+        <v>0.5</v>
       </c>
       <c r="O6">
-        <v>0.7</v>
-      </c>
-      <c r="P6" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q6">
         <v>0.5</v>
       </c>
       <c r="S6">
-        <v>0.5</v>
-      </c>
-      <c r="U6">
-        <v>0.5</v>
-      </c>
-      <c r="W6">
-        <v>0.5</v>
-      </c>
-      <c r="AA6">
         <v>5.1734967222388608</v>
       </c>
-      <c r="AB6">
+      <c r="T6">
         <f>1/0.96</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="AC6">
+      <c r="U6">
         <v>4.32</v>
       </c>
-      <c r="AF6">
+      <c r="X6">
         <v>4.45</v>
       </c>
-      <c r="AM6" s="3"/>
-      <c r="AN6" s="3"/>
-      <c r="AO6" s="5">
+      <c r="AE6" s="3"/>
+      <c r="AF6" s="3"/>
+      <c r="AG6" s="5">
         <v>0</v>
       </c>
-      <c r="AP6" s="2"/>
-    </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="AH6" s="2"/>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G7">
-        <v>100</v>
+        <v>44</v>
+      </c>
+      <c r="S7">
+        <v>7.2437800000000002E-4</v>
+      </c>
+      <c r="T7">
+        <v>0.99</v>
+      </c>
+      <c r="X7">
+        <v>0.11929223744292237</v>
       </c>
       <c r="AA7">
-        <v>7.2437800000000002E-4</v>
-      </c>
-      <c r="AB7">
-        <v>0.99</v>
-      </c>
-      <c r="AF7">
-        <v>0.11929223744292237</v>
-      </c>
-      <c r="AI7">
         <v>1.4865951742627345E-3</v>
       </c>
-      <c r="AM7" s="3"/>
-      <c r="AN7" s="3"/>
-      <c r="AO7" s="5">
+      <c r="AE7" s="3"/>
+      <c r="AF7" s="3"/>
+      <c r="AG7" s="5">
         <v>0</v>
       </c>
-      <c r="AP7" s="2"/>
+      <c r="AH7" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2:AM7" xr:uid="{D92CB468-B7A9-4082-9B81-D3B4634F286E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE2:AE7" xr:uid="{D92CB468-B7A9-4082-9B81-D3B4634F286E}">
       <formula1>"h, D, W, M, Q, Y"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1437,10 +1358,10 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1455,7 +1376,7 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
@@ -1473,72 +1394,72 @@
         <v>9</v>
       </c>
       <c r="M1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" t="s">
         <v>52</v>
       </c>
-      <c r="N1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" t="s">
         <v>53</v>
       </c>
-      <c r="Q1" t="s">
-        <v>23</v>
-      </c>
-      <c r="R1" t="s">
-        <v>24</v>
-      </c>
-      <c r="S1" t="s">
-        <v>25</v>
-      </c>
-      <c r="T1" t="s">
-        <v>54</v>
-      </c>
       <c r="U1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V1" t="s">
+        <v>28</v>
+      </c>
+      <c r="W1" t="s">
         <v>29</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>30</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>31</v>
       </c>
-      <c r="Y1" t="s">
-        <v>32</v>
-      </c>
       <c r="Z1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AA1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" t="s">
         <v>55</v>
       </c>
-      <c r="B2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" t="s">
         <v>56</v>
-      </c>
-      <c r="D2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G2" t="s">
-        <v>57</v>
       </c>
       <c r="H2">
         <v>1000</v>
@@ -1571,7 +1492,7 @@
         <v>1</v>
       </c>
       <c r="Z2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AA2">
         <v>1</v>
@@ -1579,25 +1500,25 @@
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
         <v>58</v>
       </c>
-      <c r="B3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" t="s">
-        <v>59</v>
-      </c>
       <c r="E3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H3">
         <v>1000</v>
@@ -1627,7 +1548,7 @@
         <v>7.2835616438356163E-2</v>
       </c>
       <c r="Z3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA3">
         <v>1</v>
@@ -1635,25 +1556,25 @@
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" t="s">
         <v>60</v>
       </c>
-      <c r="B4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" t="s">
-        <v>61</v>
-      </c>
       <c r="E4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H4">
         <v>1000</v>
@@ -1683,7 +1604,7 @@
         <v>1.0958904109589041E-2</v>
       </c>
       <c r="Z4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA4">
         <v>1</v>
@@ -1691,19 +1612,19 @@
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" t="s">
         <v>62</v>
       </c>
-      <c r="B5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>63</v>
-      </c>
-      <c r="G5" t="s">
-        <v>64</v>
       </c>
       <c r="H5">
         <v>1000</v>
@@ -1721,7 +1642,7 @@
         <v>1</v>
       </c>
       <c r="Z5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AA5">
         <v>1</v>
@@ -1776,51 +1697,51 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
         <v>65</v>
       </c>
-      <c r="B1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>66</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>67</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>68</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>69</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>70</v>
       </c>
-      <c r="H1" t="s">
-        <v>71</v>
-      </c>
       <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
         <v>26</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>27</v>
       </c>
-      <c r="K1" t="s">
-        <v>28</v>
-      </c>
       <c r="L1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1835,7 +1756,7 @@
         <v>4.147E-2</v>
       </c>
       <c r="H2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -1846,10 +1767,10 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1864,7 +1785,7 @@
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -1914,92 +1835,92 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Error: Mapping still not working in all cases
Work to be done but could not be finished today
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base_methanol.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base_methanol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2B69A3F-4DB4-48FC-ADEA-E31E281CE886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9013100-4C42-4BB8-9E60-3946998485A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
@@ -941,8 +941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:AH7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V3" sqref="V3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1078,10 +1078,6 @@
       </c>
       <c r="E2" t="s">
         <v>34</v>
-      </c>
-      <c r="V2" t="e">
-        <f>#REF!*0.56</f>
-        <v>#REF!</v>
       </c>
       <c r="X2">
         <v>1.29</v>

</xml_diff>

<commit_message>
Enforce product selection in main document
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base_methanol.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base_methanol.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/methanol/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9013100-4C42-4BB8-9E60-3946998485A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="13_ncr:1_{B9013100-4C42-4BB8-9E60-3946998485A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E6D3849-294E-43FB-A880-05E4309056F9}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Drop_Down" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="CIQWBGuid" hidden="1">"3701cb1e-3b63-4ab2-a684-fdb01043e14d"</definedName>
+    <definedName name="CIQWBGuid" hidden="1">"3bffc8c9-0f80-41c6-8754-51419ab314eb"</definedName>
     <definedName name="CIQWBInfo" hidden="1">"{ ""CIQVersion"":""9.51.3510.3078"" }"</definedName>
     <definedName name="IQ_CH">110000</definedName>
     <definedName name="IQ_CQ">5000</definedName>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="102">
   <si>
     <t>Unit</t>
   </si>
@@ -174,9 +174,6 @@
     <t>minimum_op_point</t>
   </si>
   <si>
-    <t>Error messages:</t>
-  </si>
-  <si>
     <t>Power_Kasso</t>
   </si>
   <si>
@@ -376,9 +373,6 @@
   </si>
   <si>
     <t>shut_down_cost</t>
-  </si>
-  <si>
-    <t>initial_units_invested_available</t>
   </si>
   <si>
     <t>initial_connections_invested_available</t>
@@ -391,7 +385,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -404,24 +398,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -444,22 +420,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="5">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -473,42 +446,6 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
     </dxf>
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -529,10 +466,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:AH7" totalsRowShown="0">
-  <autoFilter ref="A1:AH7" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
-  <tableColumns count="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:AF7" totalsRowShown="0">
+  <autoFilter ref="A1:AF7" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
+  <tableColumns count="32">
     <tableColumn id="1" xr3:uid="{C73E51D0-1842-42F3-9C00-F0DBD2E661BE}" name="Unit"/>
     <tableColumn id="40" xr3:uid="{C2CFC5A4-5329-4F74-926A-18CEB18C062C}" name="Object_type"/>
     <tableColumn id="2" xr3:uid="{FA8BE796-DE15-407E-8998-92C973AE35A4}" name="Input1"/>
@@ -563,10 +504,8 @@
     <tableColumn id="22" xr3:uid="{3FA572AD-B473-45F7-A244-2DF38E57A2D3}" name="vom_cost_Output1"/>
     <tableColumn id="23" xr3:uid="{1F97C2CD-E522-4842-8E10-F9B9566A6723}" name="vom_cost_Output2"/>
     <tableColumn id="34" xr3:uid="{7D7F0E89-0553-40E4-9D5A-219BF1741787}" name="minimum_op_point"/>
-    <tableColumn id="38" xr3:uid="{957AF85B-8792-4643-A381-29FACAA69887}" name="resolution_output" dataDxfId="6"/>
-    <tableColumn id="39" xr3:uid="{BCE2350E-150B-4A7E-94BF-BB3BC7E31016}" name="demand" dataDxfId="5"/>
-    <tableColumn id="43" xr3:uid="{4079FBE2-CFC5-4BCF-9353-8F6771C73DD2}" name="initial_units_invested_available" dataDxfId="4"/>
-    <tableColumn id="45" xr3:uid="{4B3B8871-E458-49D5-BFE4-E2DD849EE6AD}" name="Error messages:" dataDxfId="3"/>
+    <tableColumn id="38" xr3:uid="{957AF85B-8792-4643-A381-29FACAA69887}" name="resolution_output" dataDxfId="4"/>
+    <tableColumn id="39" xr3:uid="{BCE2350E-150B-4A7E-94BF-BB3BC7E31016}" name="demand" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -939,10 +878,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
-  <dimension ref="A1:AH7"/>
+  <dimension ref="A1:AF7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V3" sqref="V3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AI9" sqref="AI9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -962,15 +901,14 @@
     <col min="28" max="28" width="8.7265625" customWidth="1"/>
     <col min="31" max="31" width="18.54296875" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="10" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="17.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1015,10 +953,10 @@
         <v>21</v>
       </c>
       <c r="Q1" t="s">
+        <v>98</v>
+      </c>
+      <c r="R1" t="s">
         <v>99</v>
-      </c>
-      <c r="R1" t="s">
-        <v>100</v>
       </c>
       <c r="S1" t="s">
         <v>22</v>
@@ -1033,7 +971,7 @@
         <v>25</v>
       </c>
       <c r="W1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="X1" t="s">
         <v>26</v>
@@ -1057,56 +995,46 @@
         <v>32</v>
       </c>
       <c r="AE1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AF1" t="s">
         <v>72</v>
       </c>
-      <c r="AF1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>101</v>
-      </c>
-      <c r="AH1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E2" t="s">
-        <v>34</v>
       </c>
       <c r="X2">
         <v>1.29</v>
       </c>
-      <c r="AE2" s="3"/>
-      <c r="AF2" s="3"/>
-      <c r="AG2" s="5">
-        <v>0</v>
-      </c>
-      <c r="AH2" s="2"/>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
         <v>35</v>
       </c>
-      <c r="B3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>36</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>37</v>
-      </c>
-      <c r="F3" t="s">
-        <v>38</v>
       </c>
       <c r="G3">
         <v>0.75</v>
@@ -1126,28 +1054,24 @@
       <c r="AD3">
         <v>0.02</v>
       </c>
-      <c r="AE3" s="3"/>
-      <c r="AF3" s="3"/>
-      <c r="AG3" s="5">
-        <v>0</v>
-      </c>
-      <c r="AH3" s="2"/>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AE3" s="1"/>
+      <c r="AF3" s="1"/>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
         <v>39</v>
       </c>
-      <c r="B4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>40</v>
-      </c>
-      <c r="E4" t="s">
-        <v>41</v>
       </c>
       <c r="S4">
         <v>3.529412E-3</v>
@@ -1158,28 +1082,24 @@
       <c r="Z4">
         <v>26.81</v>
       </c>
-      <c r="AE4" s="3"/>
-      <c r="AF4" s="3"/>
-      <c r="AG4" s="5">
-        <v>0</v>
-      </c>
-      <c r="AH4" s="2"/>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AE4" s="1"/>
+      <c r="AF4" s="1"/>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" t="s">
         <v>42</v>
       </c>
-      <c r="B5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>43</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>44</v>
-      </c>
-      <c r="E5" t="s">
-        <v>45</v>
       </c>
       <c r="S5">
         <v>17.277901743828668</v>
@@ -1188,41 +1108,37 @@
         <f>1/0.795</f>
         <v>1.2578616352201257</v>
       </c>
-      <c r="AE5" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AF5" s="4">
+      <c r="AE5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AF5" s="2">
         <v>20.192799999999998</v>
       </c>
-      <c r="AG5" s="5">
-        <v>0</v>
-      </c>
-      <c r="AH5" s="2"/>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" t="s">
         <v>37</v>
-      </c>
-      <c r="D6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" t="s">
-        <v>43</v>
-      </c>
-      <c r="F6" t="s">
-        <v>38</v>
       </c>
       <c r="G6">
         <v>0.7</v>
       </c>
       <c r="H6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I6">
         <v>0.5</v>
@@ -1249,28 +1165,24 @@
       <c r="X6">
         <v>4.45</v>
       </c>
-      <c r="AE6" s="3"/>
-      <c r="AF6" s="3"/>
-      <c r="AG6" s="5">
-        <v>0</v>
-      </c>
-      <c r="AH6" s="2"/>
-    </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AE6" s="1"/>
+      <c r="AF6" s="1"/>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="S7">
         <v>7.2437800000000002E-4</v>
@@ -1284,12 +1196,8 @@
       <c r="AA7">
         <v>1.4865951742627345E-3</v>
       </c>
-      <c r="AE7" s="3"/>
-      <c r="AF7" s="3"/>
-      <c r="AG7" s="5">
-        <v>0</v>
-      </c>
-      <c r="AH7" s="2"/>
+      <c r="AE7" s="1"/>
+      <c r="AF7" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1354,10 +1262,10 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1372,7 +1280,7 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
@@ -1390,7 +1298,7 @@
         <v>9</v>
       </c>
       <c r="M1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N1" t="s">
         <v>10</v>
@@ -1399,7 +1307,7 @@
         <v>11</v>
       </c>
       <c r="P1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Q1" t="s">
         <v>22</v>
@@ -1411,7 +1319,7 @@
         <v>24</v>
       </c>
       <c r="T1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="U1" t="s">
         <v>26</v>
@@ -1429,33 +1337,33 @@
         <v>31</v>
       </c>
       <c r="Z1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AA1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" t="s">
         <v>54</v>
       </c>
-      <c r="B2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" t="s">
         <v>55</v>
-      </c>
-      <c r="D2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G2" t="s">
-        <v>56</v>
       </c>
       <c r="H2">
         <v>1000</v>
@@ -1488,7 +1396,7 @@
         <v>1</v>
       </c>
       <c r="Z2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA2">
         <v>1</v>
@@ -1496,25 +1404,25 @@
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" t="s">
         <v>57</v>
       </c>
-      <c r="B3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" t="s">
-        <v>58</v>
-      </c>
       <c r="E3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H3">
         <v>1000</v>
@@ -1544,7 +1452,7 @@
         <v>7.2835616438356163E-2</v>
       </c>
       <c r="Z3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AA3">
         <v>1</v>
@@ -1552,25 +1460,25 @@
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" t="s">
         <v>59</v>
       </c>
-      <c r="B4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" t="s">
-        <v>60</v>
-      </c>
       <c r="E4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H4">
         <v>1000</v>
@@ -1600,7 +1508,7 @@
         <v>1.0958904109589041E-2</v>
       </c>
       <c r="Z4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AA4">
         <v>1</v>
@@ -1608,19 +1516,19 @@
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" t="s">
         <v>61</v>
       </c>
-      <c r="B5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>62</v>
-      </c>
-      <c r="G5" t="s">
-        <v>63</v>
       </c>
       <c r="H5">
         <v>1000</v>
@@ -1638,7 +1546,7 @@
         <v>1</v>
       </c>
       <c r="Z5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA5">
         <v>1</v>
@@ -1693,28 +1601,28 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" t="s">
         <v>64</v>
       </c>
-      <c r="B1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>65</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>66</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>67</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>68</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>69</v>
-      </c>
-      <c r="H1" t="s">
-        <v>70</v>
       </c>
       <c r="I1" t="s">
         <v>25</v>
@@ -1726,18 +1634,18 @@
         <v>27</v>
       </c>
       <c r="L1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="M1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1752,7 +1660,7 @@
         <v>4.147E-2</v>
       </c>
       <c r="H2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -1763,10 +1671,10 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1781,7 +1689,7 @@
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -1821,7 +1729,7 @@
   <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1831,92 +1739,92 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Enforce product selection in main document"
This reverts commit a5662f19e2e545da8b548c28fb6e36c7e7d15918.
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base_methanol.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base_methanol.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/methanol/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="13_ncr:1_{B9013100-4C42-4BB8-9E60-3946998485A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E6D3849-294E-43FB-A880-05E4309056F9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9013100-4C42-4BB8-9E60-3946998485A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Drop_Down" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="CIQWBGuid" hidden="1">"3bffc8c9-0f80-41c6-8754-51419ab314eb"</definedName>
+    <definedName name="CIQWBGuid" hidden="1">"3701cb1e-3b63-4ab2-a684-fdb01043e14d"</definedName>
     <definedName name="CIQWBInfo" hidden="1">"{ ""CIQVersion"":""9.51.3510.3078"" }"</definedName>
     <definedName name="IQ_CH">110000</definedName>
     <definedName name="IQ_CQ">5000</definedName>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="104">
   <si>
     <t>Unit</t>
   </si>
@@ -174,6 +174,9 @@
     <t>minimum_op_point</t>
   </si>
   <si>
+    <t>Error messages:</t>
+  </si>
+  <si>
     <t>Power_Kasso</t>
   </si>
   <si>
@@ -373,6 +376,9 @@
   </si>
   <si>
     <t>shut_down_cost</t>
+  </si>
+  <si>
+    <t>initial_units_invested_available</t>
   </si>
   <si>
     <t>initial_connections_invested_available</t>
@@ -385,7 +391,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -398,6 +404,24 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -420,19 +444,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="7">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -446,6 +473,42 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -466,14 +529,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:AF7" totalsRowShown="0">
-  <autoFilter ref="A1:AF7" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
-  <tableColumns count="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:AH7" totalsRowShown="0">
+  <autoFilter ref="A1:AH7" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
+  <tableColumns count="34">
     <tableColumn id="1" xr3:uid="{C73E51D0-1842-42F3-9C00-F0DBD2E661BE}" name="Unit"/>
     <tableColumn id="40" xr3:uid="{C2CFC5A4-5329-4F74-926A-18CEB18C062C}" name="Object_type"/>
     <tableColumn id="2" xr3:uid="{FA8BE796-DE15-407E-8998-92C973AE35A4}" name="Input1"/>
@@ -504,8 +563,10 @@
     <tableColumn id="22" xr3:uid="{3FA572AD-B473-45F7-A244-2DF38E57A2D3}" name="vom_cost_Output1"/>
     <tableColumn id="23" xr3:uid="{1F97C2CD-E522-4842-8E10-F9B9566A6723}" name="vom_cost_Output2"/>
     <tableColumn id="34" xr3:uid="{7D7F0E89-0553-40E4-9D5A-219BF1741787}" name="minimum_op_point"/>
-    <tableColumn id="38" xr3:uid="{957AF85B-8792-4643-A381-29FACAA69887}" name="resolution_output" dataDxfId="4"/>
-    <tableColumn id="39" xr3:uid="{BCE2350E-150B-4A7E-94BF-BB3BC7E31016}" name="demand" dataDxfId="3"/>
+    <tableColumn id="38" xr3:uid="{957AF85B-8792-4643-A381-29FACAA69887}" name="resolution_output" dataDxfId="6"/>
+    <tableColumn id="39" xr3:uid="{BCE2350E-150B-4A7E-94BF-BB3BC7E31016}" name="demand" dataDxfId="5"/>
+    <tableColumn id="43" xr3:uid="{4079FBE2-CFC5-4BCF-9353-8F6771C73DD2}" name="initial_units_invested_available" dataDxfId="4"/>
+    <tableColumn id="45" xr3:uid="{4B3B8871-E458-49D5-BFE4-E2DD849EE6AD}" name="Error messages:" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -878,10 +939,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
-  <dimension ref="A1:AF7"/>
+  <dimension ref="A1:AH7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AI9" sqref="AI9"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V3" sqref="V3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -901,14 +962,15 @@
     <col min="28" max="28" width="8.7265625" customWidth="1"/>
     <col min="31" max="31" width="18.54296875" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="10" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="17.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -953,10 +1015,10 @@
         <v>21</v>
       </c>
       <c r="Q1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="R1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="S1" t="s">
         <v>22</v>
@@ -971,7 +1033,7 @@
         <v>25</v>
       </c>
       <c r="W1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="X1" t="s">
         <v>26</v>
@@ -995,46 +1057,56 @@
         <v>32</v>
       </c>
       <c r="AE1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="AF1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
+        <v>73</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="X2">
         <v>1.29</v>
       </c>
-      <c r="AE2" s="1"/>
-      <c r="AF2" s="1"/>
-    </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AE2" s="3"/>
+      <c r="AF2" s="3"/>
+      <c r="AG2" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="2"/>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" t="s">
         <v>34</v>
       </c>
-      <c r="B3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C3" t="s">
-        <v>33</v>
-      </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G3">
         <v>0.75</v>
@@ -1054,24 +1126,28 @@
       <c r="AD3">
         <v>0.02</v>
       </c>
-      <c r="AE3" s="1"/>
-      <c r="AF3" s="1"/>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AE3" s="3"/>
+      <c r="AF3" s="3"/>
+      <c r="AG3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH3" s="2"/>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="S4">
         <v>3.529412E-3</v>
@@ -1082,24 +1158,28 @@
       <c r="Z4">
         <v>26.81</v>
       </c>
-      <c r="AE4" s="1"/>
-      <c r="AF4" s="1"/>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AE4" s="3"/>
+      <c r="AF4" s="3"/>
+      <c r="AG4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="2"/>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="S5">
         <v>17.277901743828668</v>
@@ -1108,37 +1188,41 @@
         <f>1/0.795</f>
         <v>1.2578616352201257</v>
       </c>
-      <c r="AE5" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AF5" s="2">
+      <c r="AE5" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AF5" s="4">
         <v>20.192799999999998</v>
       </c>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AG5" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH5" s="2"/>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G6">
         <v>0.7</v>
       </c>
       <c r="H6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I6">
         <v>0.5</v>
@@ -1165,24 +1249,28 @@
       <c r="X6">
         <v>4.45</v>
       </c>
-      <c r="AE6" s="1"/>
-      <c r="AF6" s="1"/>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AE6" s="3"/>
+      <c r="AF6" s="3"/>
+      <c r="AG6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH6" s="2"/>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="S7">
         <v>7.2437800000000002E-4</v>
@@ -1196,8 +1284,12 @@
       <c r="AA7">
         <v>1.4865951742627345E-3</v>
       </c>
-      <c r="AE7" s="1"/>
-      <c r="AF7" s="1"/>
+      <c r="AE7" s="3"/>
+      <c r="AF7" s="3"/>
+      <c r="AG7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH7" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1262,10 +1354,10 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1280,7 +1372,7 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
@@ -1298,7 +1390,7 @@
         <v>9</v>
       </c>
       <c r="M1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N1" t="s">
         <v>10</v>
@@ -1307,7 +1399,7 @@
         <v>11</v>
       </c>
       <c r="P1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="Q1" t="s">
         <v>22</v>
@@ -1319,7 +1411,7 @@
         <v>24</v>
       </c>
       <c r="T1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="U1" t="s">
         <v>26</v>
@@ -1337,33 +1429,33 @@
         <v>31</v>
       </c>
       <c r="Z1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AA1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H2">
         <v>1000</v>
@@ -1396,7 +1488,7 @@
         <v>1</v>
       </c>
       <c r="Z2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AA2">
         <v>1</v>
@@ -1404,25 +1496,25 @@
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H3">
         <v>1000</v>
@@ -1452,7 +1544,7 @@
         <v>7.2835616438356163E-2</v>
       </c>
       <c r="Z3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AA3">
         <v>1</v>
@@ -1460,25 +1552,25 @@
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H4">
         <v>1000</v>
@@ -1508,7 +1600,7 @@
         <v>1.0958904109589041E-2</v>
       </c>
       <c r="Z4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AA4">
         <v>1</v>
@@ -1516,19 +1608,19 @@
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H5">
         <v>1000</v>
@@ -1546,7 +1638,7 @@
         <v>1</v>
       </c>
       <c r="Z5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AA5">
         <v>1</v>
@@ -1601,28 +1693,28 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I1" t="s">
         <v>25</v>
@@ -1634,18 +1726,18 @@
         <v>27</v>
       </c>
       <c r="L1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="M1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1660,7 +1752,7 @@
         <v>4.147E-2</v>
       </c>
       <c r="H2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -1671,10 +1763,10 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1689,7 +1781,7 @@
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -1729,7 +1821,7 @@
   <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1739,92 +1831,92 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added capacities if minimum op point is used
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base_methanol.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base_methanol.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/methanol/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9013100-4C42-4BB8-9E60-3946998485A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:1_{B9013100-4C42-4BB8-9E60-3946998485A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9AB8DAFF-AE66-454B-BCBF-C6B62A26B841}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="102">
   <si>
     <t>Unit</t>
   </si>
@@ -174,9 +174,6 @@
     <t>minimum_op_point</t>
   </si>
   <si>
-    <t>Error messages:</t>
-  </si>
-  <si>
     <t>Power_Kasso</t>
   </si>
   <si>
@@ -376,9 +373,6 @@
   </si>
   <si>
     <t>shut_down_cost</t>
-  </si>
-  <si>
-    <t>initial_units_invested_available</t>
   </si>
   <si>
     <t>initial_connections_invested_available</t>
@@ -391,7 +385,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -404,24 +398,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -444,22 +420,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="5">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -473,42 +446,6 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
     </dxf>
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -530,9 +467,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:AH7" totalsRowShown="0">
-  <autoFilter ref="A1:AH7" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
-  <tableColumns count="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:AF7" totalsRowShown="0">
+  <autoFilter ref="A1:AF7" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
+  <tableColumns count="32">
     <tableColumn id="1" xr3:uid="{C73E51D0-1842-42F3-9C00-F0DBD2E661BE}" name="Unit"/>
     <tableColumn id="40" xr3:uid="{C2CFC5A4-5329-4F74-926A-18CEB18C062C}" name="Object_type"/>
     <tableColumn id="2" xr3:uid="{FA8BE796-DE15-407E-8998-92C973AE35A4}" name="Input1"/>
@@ -563,10 +500,8 @@
     <tableColumn id="22" xr3:uid="{3FA572AD-B473-45F7-A244-2DF38E57A2D3}" name="vom_cost_Output1"/>
     <tableColumn id="23" xr3:uid="{1F97C2CD-E522-4842-8E10-F9B9566A6723}" name="vom_cost_Output2"/>
     <tableColumn id="34" xr3:uid="{7D7F0E89-0553-40E4-9D5A-219BF1741787}" name="minimum_op_point"/>
-    <tableColumn id="38" xr3:uid="{957AF85B-8792-4643-A381-29FACAA69887}" name="resolution_output" dataDxfId="6"/>
-    <tableColumn id="39" xr3:uid="{BCE2350E-150B-4A7E-94BF-BB3BC7E31016}" name="demand" dataDxfId="5"/>
-    <tableColumn id="43" xr3:uid="{4079FBE2-CFC5-4BCF-9353-8F6771C73DD2}" name="initial_units_invested_available" dataDxfId="4"/>
-    <tableColumn id="45" xr3:uid="{4B3B8871-E458-49D5-BFE4-E2DD849EE6AD}" name="Error messages:" dataDxfId="3"/>
+    <tableColumn id="38" xr3:uid="{957AF85B-8792-4643-A381-29FACAA69887}" name="resolution_output" dataDxfId="4"/>
+    <tableColumn id="39" xr3:uid="{BCE2350E-150B-4A7E-94BF-BB3BC7E31016}" name="demand" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -939,10 +874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
-  <dimension ref="A1:AH7"/>
+  <dimension ref="A1:AF7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V3" sqref="V3"/>
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AD15" sqref="AD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -962,15 +897,14 @@
     <col min="28" max="28" width="8.7265625" customWidth="1"/>
     <col min="31" max="31" width="18.54296875" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="10" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="17.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1015,10 +949,10 @@
         <v>21</v>
       </c>
       <c r="Q1" t="s">
+        <v>98</v>
+      </c>
+      <c r="R1" t="s">
         <v>99</v>
-      </c>
-      <c r="R1" t="s">
-        <v>100</v>
       </c>
       <c r="S1" t="s">
         <v>22</v>
@@ -1033,7 +967,7 @@
         <v>25</v>
       </c>
       <c r="W1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="X1" t="s">
         <v>26</v>
@@ -1057,56 +991,46 @@
         <v>32</v>
       </c>
       <c r="AE1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AF1" t="s">
         <v>72</v>
       </c>
-      <c r="AF1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>101</v>
-      </c>
-      <c r="AH1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E2" t="s">
-        <v>34</v>
       </c>
       <c r="X2">
         <v>1.29</v>
       </c>
-      <c r="AE2" s="3"/>
-      <c r="AF2" s="3"/>
-      <c r="AG2" s="5">
-        <v>0</v>
-      </c>
-      <c r="AH2" s="2"/>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
         <v>35</v>
       </c>
-      <c r="B3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>36</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>37</v>
-      </c>
-      <c r="F3" t="s">
-        <v>38</v>
       </c>
       <c r="G3">
         <v>0.75</v>
@@ -1126,28 +1050,24 @@
       <c r="AD3">
         <v>0.02</v>
       </c>
-      <c r="AE3" s="3"/>
-      <c r="AF3" s="3"/>
-      <c r="AG3" s="5">
-        <v>0</v>
-      </c>
-      <c r="AH3" s="2"/>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AE3" s="1"/>
+      <c r="AF3" s="1"/>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
         <v>39</v>
       </c>
-      <c r="B4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>40</v>
-      </c>
-      <c r="E4" t="s">
-        <v>41</v>
       </c>
       <c r="S4">
         <v>3.529412E-3</v>
@@ -1158,28 +1078,24 @@
       <c r="Z4">
         <v>26.81</v>
       </c>
-      <c r="AE4" s="3"/>
-      <c r="AF4" s="3"/>
-      <c r="AG4" s="5">
-        <v>0</v>
-      </c>
-      <c r="AH4" s="2"/>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AE4" s="1"/>
+      <c r="AF4" s="1"/>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" t="s">
         <v>42</v>
       </c>
-      <c r="B5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>43</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>44</v>
-      </c>
-      <c r="E5" t="s">
-        <v>45</v>
       </c>
       <c r="S5">
         <v>17.277901743828668</v>
@@ -1188,41 +1104,37 @@
         <f>1/0.795</f>
         <v>1.2578616352201257</v>
       </c>
-      <c r="AE5" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AF5" s="4">
+      <c r="AE5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AF5" s="2">
         <v>20.192799999999998</v>
       </c>
-      <c r="AG5" s="5">
-        <v>0</v>
-      </c>
-      <c r="AH5" s="2"/>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" t="s">
         <v>37</v>
-      </c>
-      <c r="D6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" t="s">
-        <v>43</v>
-      </c>
-      <c r="F6" t="s">
-        <v>38</v>
       </c>
       <c r="G6">
         <v>0.7</v>
       </c>
       <c r="H6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I6">
         <v>0.5</v>
@@ -1249,28 +1161,24 @@
       <c r="X6">
         <v>4.45</v>
       </c>
-      <c r="AE6" s="3"/>
-      <c r="AF6" s="3"/>
-      <c r="AG6" s="5">
-        <v>0</v>
-      </c>
-      <c r="AH6" s="2"/>
-    </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AE6" s="1"/>
+      <c r="AF6" s="1"/>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="S7">
         <v>7.2437800000000002E-4</v>
@@ -1284,12 +1192,8 @@
       <c r="AA7">
         <v>1.4865951742627345E-3</v>
       </c>
-      <c r="AE7" s="3"/>
-      <c r="AF7" s="3"/>
-      <c r="AG7" s="5">
-        <v>0</v>
-      </c>
-      <c r="AH7" s="2"/>
+      <c r="AE7" s="1"/>
+      <c r="AF7" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1354,10 +1258,10 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1372,7 +1276,7 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
@@ -1390,7 +1294,7 @@
         <v>9</v>
       </c>
       <c r="M1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N1" t="s">
         <v>10</v>
@@ -1399,7 +1303,7 @@
         <v>11</v>
       </c>
       <c r="P1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Q1" t="s">
         <v>22</v>
@@ -1411,7 +1315,7 @@
         <v>24</v>
       </c>
       <c r="T1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="U1" t="s">
         <v>26</v>
@@ -1429,33 +1333,33 @@
         <v>31</v>
       </c>
       <c r="Z1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AA1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" t="s">
         <v>54</v>
       </c>
-      <c r="B2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" t="s">
         <v>55</v>
-      </c>
-      <c r="D2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G2" t="s">
-        <v>56</v>
       </c>
       <c r="H2">
         <v>1000</v>
@@ -1488,7 +1392,7 @@
         <v>1</v>
       </c>
       <c r="Z2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA2">
         <v>1</v>
@@ -1496,25 +1400,25 @@
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" t="s">
         <v>57</v>
       </c>
-      <c r="B3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" t="s">
-        <v>58</v>
-      </c>
       <c r="E3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H3">
         <v>1000</v>
@@ -1544,7 +1448,7 @@
         <v>7.2835616438356163E-2</v>
       </c>
       <c r="Z3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AA3">
         <v>1</v>
@@ -1552,25 +1456,25 @@
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" t="s">
         <v>59</v>
       </c>
-      <c r="B4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" t="s">
-        <v>60</v>
-      </c>
       <c r="E4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H4">
         <v>1000</v>
@@ -1600,7 +1504,7 @@
         <v>1.0958904109589041E-2</v>
       </c>
       <c r="Z4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AA4">
         <v>1</v>
@@ -1608,19 +1512,19 @@
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" t="s">
         <v>61</v>
       </c>
-      <c r="B5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>62</v>
-      </c>
-      <c r="G5" t="s">
-        <v>63</v>
       </c>
       <c r="H5">
         <v>1000</v>
@@ -1638,7 +1542,7 @@
         <v>1</v>
       </c>
       <c r="Z5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA5">
         <v>1</v>
@@ -1693,28 +1597,28 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" t="s">
         <v>64</v>
       </c>
-      <c r="B1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>65</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>66</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>67</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>68</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>69</v>
-      </c>
-      <c r="H1" t="s">
-        <v>70</v>
       </c>
       <c r="I1" t="s">
         <v>25</v>
@@ -1726,18 +1630,18 @@
         <v>27</v>
       </c>
       <c r="L1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="M1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1752,7 +1656,7 @@
         <v>4.147E-2</v>
       </c>
       <c r="H2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -1763,10 +1667,10 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1781,7 +1685,7 @@
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -1831,92 +1735,92 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update for added unit__to/from_node definitions
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base_methanol.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base_methanol.xlsx
@@ -876,8 +876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:AF7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AD15" sqref="AD15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
remove not necessary links to power
not all units need power supply in the current implementation.
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base_methanol.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base_methanol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0C441B8-6EC6-4057-8A48-93EB696D7A65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E50A2FE-790C-4315-A225-4A5016C0D528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4590" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
@@ -896,7 +896,7 @@
   <dimension ref="A1:AJ7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1127,12 +1127,6 @@
       </c>
       <c r="E5" t="s">
         <v>92</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
       </c>
       <c r="S5">
         <v>17.277901743828668</v>

</xml_diff>

<commit_message>
fix node state bug for hours that do not have a min node state
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base_methanol.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base_methanol.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/methanol/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{7E50A2FE-790C-4315-A225-4A5016C0D528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{28236D91-BD55-4766-B14C-B21F53D67A9F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A0FF428-631D-45E7-A1AB-2AAD8B828C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22815" yWindow="-21720" windowWidth="51840" windowHeight="21240" activeTab="2" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -891,8 +891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:AJ7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X3" sqref="X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1035,7 +1035,7 @@
         <v>80</v>
       </c>
       <c r="X2">
-        <v>1.29</v>
+        <v>0</v>
       </c>
       <c r="AI2" s="1"/>
       <c r="AJ2" s="1"/>
@@ -1601,7 +1601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{981CFA5E-60F3-446F-A856-2FA65B76879A}">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added option for demand (+ resolution)
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base_methanol.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base_methanol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/methanol/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{3A0FF428-631D-45E7-A1AB-2AAD8B828C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66C9D0C5-DBD6-479D-B366-E24ED1417B90}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="13_ncr:1_{3A0FF428-631D-45E7-A1AB-2AAD8B828C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A82C1248-9E41-4884-A09A-D12B48DDEEE7}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
@@ -483,8 +483,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:AK7" totalsRowShown="0">
-  <autoFilter ref="A1:AK7" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:AK8" totalsRowShown="0">
+  <autoFilter ref="A1:AK8" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
   <tableColumns count="37">
     <tableColumn id="1" xr3:uid="{C73E51D0-1842-42F3-9C00-F0DBD2E661BE}" name="Unit"/>
     <tableColumn id="40" xr3:uid="{C2CFC5A4-5329-4F74-926A-18CEB18C062C}" name="Object_type"/>
@@ -893,11 +893,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
-  <dimension ref="A1:AK7"/>
+  <dimension ref="A1:AK8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AK7" sqref="AK7"/>
+      <selection pane="topRight" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1233,10 +1233,14 @@
       <c r="AI7" s="1"/>
       <c r="AJ7" s="1"/>
     </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.35">
+      <c r="AI8" s="1"/>
+      <c r="AJ8" s="1"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI2:AI7" xr:uid="{D92CB468-B7A9-4082-9B81-D3B4634F286E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI2:AI8" xr:uid="{D92CB468-B7A9-4082-9B81-D3B4634F286E}">
       <formula1>"h, D, W, M, Q, Y"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1264,7 +1268,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C870BDA0-9E4C-481D-87BE-9D47789809C8}">
   <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S5" sqref="S5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>